<commit_message>
se agrego wait time en el excel,acciones wait,implicitlyWait,compare esta en proceso
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Training\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Training\Desktop\Prueba\frameWorkBatch3\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Accion</t>
   </si>
@@ -59,16 +59,34 @@
     <t>btnK</t>
   </si>
   <si>
-    <t>navegate</t>
-  </si>
-  <si>
     <t>https://www.google.com/</t>
   </si>
   <si>
     <t>quit</t>
   </si>
   <si>
-    <t>screenshot</t>
+    <t>navigate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait </t>
+  </si>
+  <si>
+    <t>Screenshot</t>
+  </si>
+  <si>
+    <t>Wait Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compare </t>
+  </si>
+  <si>
+    <t>hola</t>
+  </si>
+  <si>
+    <t>//div[@class='kno-ecr-pt PZPZlf gsmt i8lZMc']//span[contains(text(),'Selenium')]</t>
+  </si>
+  <si>
+    <t>xpath</t>
   </si>
 </sst>
 </file>
@@ -92,15 +110,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -108,17 +132,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -400,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,7 +453,7 @@
     <col min="4" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -430,77 +470,127 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="www.google.com"/>
-    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se arreglo la accion confirm,alert,se agrego un txt de las acciones en la carpeta de excel
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Accion</t>
   </si>
@@ -77,16 +77,13 @@
     <t>Wait Time</t>
   </si>
   <si>
-    <t xml:space="preserve">compare </t>
-  </si>
-  <si>
-    <t>hola</t>
-  </si>
-  <si>
-    <t>//div[@class='kno-ecr-pt PZPZlf gsmt i8lZMc']//span[contains(text(),'Selenium')]</t>
-  </si>
-  <si>
     <t>xpath</t>
+  </si>
+  <si>
+    <t>confirm</t>
+  </si>
+  <si>
+    <t>//body[@id='gsr']/div[@id='main']/div[@id='cnt']/div[@class='mw']/div[@id='rcnt']/div[@class='col']/div[@id='center_col']/div[@id='res']/div[@id='search']/div/div[@id='rso']/div[1]/div[1]/div[1]/div[1]/div[1]/a[1]/h3[1]</t>
   </si>
 </sst>
 </file>
@@ -443,7 +440,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +530,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -552,16 +549,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Se agrego la casilla de description en el excel
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
-  <si>
-    <t>Accion</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Locator</t>
   </si>
@@ -84,6 +81,15 @@
   </si>
   <si>
     <t>//body[@id='gsr']/div[@id='main']/div[@id='cnt']/div[@class='mw']/div[@id='rcnt']/div[@class='col']/div[@id='center_col']/div[@id='res']/div[@id='search']/div/div[@id='rso']/div[1]/div[1]/div[1]/div[1]/div[1]/a[1]/h3[1]</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Navegar a google</t>
   </si>
 </sst>
 </file>
@@ -437,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,142 +456,153 @@
     <col min="4" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E2" s="3"/>
-      <c r="F2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
se agregaron las acciones randuser y randemail se implemento un wait y se agregaron clases de la lectura de hojas(en proceso). TC2 es el main para pruebas
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="TC1" sheetId="1" r:id="rId1"/>
+    <sheet name="TC2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Locator</t>
   </si>
@@ -47,15 +48,9 @@
     <t>q</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>Selenium</t>
   </si>
   <si>
-    <t>btnK</t>
-  </si>
-  <si>
     <t>https://www.google.com/</t>
   </si>
   <si>
@@ -90,6 +85,12 @@
   </si>
   <si>
     <t>Navegar a google</t>
+  </si>
+  <si>
+    <t>randemail</t>
+  </si>
+  <si>
+    <t>//div[@class='FPdoLc tfB0Bf']//input[@name='btnK']</t>
   </si>
 </sst>
 </file>
@@ -127,7 +128,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -150,18 +151,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -443,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,10 +474,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -476,10 +489,10 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -487,13 +500,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -506,36 +519,35 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
+      <c r="B3" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="G3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H3" s="3">
-        <v>10</v>
-      </c>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>7</v>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>6</v>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
       </c>
       <c r="G4" s="3" t="b">
         <v>1</v>
@@ -546,38 +558,35 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5">
         <v>4</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="G6" s="3" t="b">
         <v>1</v>
@@ -588,17 +597,34 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
       <c r="G7" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -607,4 +633,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
SE agregaron los screenshots,ahora se leen las hojas de los excel main TC1
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TC1" sheetId="1" r:id="rId1"/>
-    <sheet name="TC2" sheetId="2" r:id="rId2"/>
+    <sheet name="TC2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>Locator</t>
   </si>
@@ -48,9 +48,6 @@
     <t>q</t>
   </si>
   <si>
-    <t>Selenium</t>
-  </si>
-  <si>
     <t>https://www.google.com/</t>
   </si>
   <si>
@@ -70,12 +67,6 @@
   </si>
   <si>
     <t>xpath</t>
-  </si>
-  <si>
-    <t>confirm</t>
-  </si>
-  <si>
-    <t>//body[@id='gsr']/div[@id='main']/div[@id='cnt']/div[@class='mw']/div[@id='rcnt']/div[@class='col']/div[@id='center_col']/div[@id='res']/div[@id='search']/div/div[@id='rso']/div[1]/div[1]/div[1]/div[1]/div[1]/a[1]/h3[1]</t>
   </si>
   <si>
     <t>Description</t>
@@ -456,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,10 +465,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -489,10 +480,10 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -500,19 +491,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="3" t="b">
-        <v>1</v>
-      </c>
+      <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -520,7 +509,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3"/>
       <c r="E3" s="5" t="s">
@@ -544,10 +533,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G4" s="3" t="b">
         <v>1</v>
@@ -559,7 +548,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="3"/>
@@ -572,59 +561,14 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="3" t="b">
-        <v>1</v>
-      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -637,14 +581,132 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrego la accion typenumeric
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>Locator</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>//div[@class='FPdoLc tfB0Bf']//input[@name='btnK']</t>
+  </si>
+  <si>
+    <t>typenumeric</t>
   </si>
 </sst>
 </file>
@@ -584,7 +587,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +641,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3"/>
       <c r="E3" s="5" t="s">
@@ -650,7 +653,9 @@
       <c r="G3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H3" s="3"/>
+      <c r="H3" s="3">
+        <v>345434</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">

</xml_diff>

<commit_message>
Se agregaron los screenshots en carpetas y el reporte base de html junto a sus screen
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="TC1" sheetId="1" r:id="rId1"/>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="A1:H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +504,9 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -570,7 +572,9 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="H6" s="3"/>
     </row>
   </sheetData>
@@ -586,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +637,9 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -705,7 +711,9 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="H6" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
el reporte se abre solo, se corrigio el tiempo de los elementos, se agrego la accion compto
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TC1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Locator</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>typenumeric</t>
+  </si>
+  <si>
+    <t>//a[contains(text(),'Gmail')]</t>
+  </si>
+  <si>
+    <t>compto</t>
+  </si>
+  <si>
+    <t>Hola</t>
   </si>
 </sst>
 </file>
@@ -452,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,10 +597,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,75 +655,95 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="E3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>6</v>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
       </c>
       <c r="G3" s="3" t="b">
         <v>1</v>
-      </c>
-      <c r="H3" s="3">
-        <v>345434</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
+      <c r="E4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="G4" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H4" s="3"/>
+      <c r="H4" s="3">
+        <v>345434</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
       <c r="G5" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="B6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H6" s="3"/>
+      <c r="H6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
se termino el reporte, se agrego el dragndrop
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="TC1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>Locator</t>
   </si>
@@ -94,6 +94,24 @@
   </si>
   <si>
     <t>Hola</t>
+  </si>
+  <si>
+    <t>Locator Value</t>
+  </si>
+  <si>
+    <t>Valor Action</t>
+  </si>
+  <si>
+    <t>Destination Locator</t>
+  </si>
+  <si>
+    <t>Destination Locator Value</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>dragndrop</t>
   </si>
 </sst>
 </file>
@@ -117,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,6 +145,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -170,13 +194,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -459,20 +485,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -483,22 +514,28 @@
         <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -513,12 +550,14 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="3" t="b">
-        <v>1</v>
-      </c>
+      <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -526,65 +565,74 @@
         <v>17</v>
       </c>
       <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3" t="b">
-        <v>1</v>
-      </c>
+      <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="3" t="b">
-        <v>1</v>
-      </c>
+      <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="6"/>
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3" t="b">
-        <v>1</v>
-      </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="3"/>
+      <c r="I6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -597,15 +645,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -624,14 +681,20 @@
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -646,32 +709,38 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="3" t="b">
-        <v>1</v>
-      </c>
+      <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -679,20 +748,23 @@
         <v>19</v>
       </c>
       <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
         <v>345434</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -704,46 +776,61 @@
       <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="3" t="b">
-        <v>1</v>
-      </c>
+      <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="3" t="b">
-        <v>1</v>
-      </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="3"/>
+      <c r="I7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
se agrego documentacion y la accion wait solos se agrega el wait time y espera antes de una excepcion
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="TC1" sheetId="1" r:id="rId1"/>
-    <sheet name="TC2" sheetId="3" r:id="rId2"/>
+    <sheet name="TC1" sheetId="3" r:id="rId1"/>
+    <sheet name="DragnDrop" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>Locator</t>
   </si>
   <si>
-    <t>Valor Locator</t>
-  </si>
-  <si>
-    <t>Valor Accion</t>
-  </si>
-  <si>
     <t>Step</t>
   </si>
   <si>
@@ -78,9 +72,6 @@
     <t>Navegar a google</t>
   </si>
   <si>
-    <t>randemail</t>
-  </si>
-  <si>
     <t>//div[@class='FPdoLc tfB0Bf']//input[@name='btnK']</t>
   </si>
   <si>
@@ -96,22 +87,31 @@
     <t>Hola</t>
   </si>
   <si>
-    <t>Locator Value</t>
-  </si>
-  <si>
-    <t>Valor Action</t>
-  </si>
-  <si>
     <t>Destination Locator</t>
   </si>
   <si>
     <t>Destination Locator Value</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>dragndrop</t>
+  </si>
+  <si>
+    <t>arrastrar</t>
+  </si>
+  <si>
+    <t>http://demo.guru99.com/test/drag_drop.html</t>
+  </si>
+  <si>
+    <t>//section[@id='g-container-main']//li[4]//a[1]</t>
+  </si>
+  <si>
+    <t>//ol[@id='bank']</t>
+  </si>
+  <si>
+    <t>Value Action</t>
+  </si>
+  <si>
+    <t>Value Locator</t>
   </si>
 </sst>
 </file>
@@ -155,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -178,23 +178,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -203,7 +192,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -485,170 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="3">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="J7" sqref="A1:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,34 +492,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -699,13 +527,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -721,17 +549,17 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -745,15 +573,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -769,15 +597,15 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -790,16 +618,24 @@
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="B6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="6"/>
@@ -814,23 +650,123 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
se agrego otra implementacion del wait
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="TC1" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>Locator</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Navegar a google</t>
   </si>
   <si>
-    <t>//div[@class='FPdoLc tfB0Bf']//input[@name='btnK']</t>
-  </si>
-  <si>
     <t>typenumeric</t>
   </si>
   <si>
@@ -112,6 +109,18 @@
   </si>
   <si>
     <t>Value Locator</t>
+  </si>
+  <si>
+    <t>hola</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>//a[contains(text(),'Realeza')]</t>
+  </si>
+  <si>
+    <t>enter</t>
   </si>
 </sst>
 </file>
@@ -473,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="A1:J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,19 +510,19 @@
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
@@ -549,17 +558,17 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -573,10 +582,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
@@ -588,24 +599,22 @@
       <c r="I4" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="3">
-        <v>345434</v>
-      </c>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -619,7 +628,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -639,16 +648,40 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="J7" s="3">
-        <v>4</v>
-      </c>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -662,7 +695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
@@ -679,19 +712,19 @@
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
@@ -711,7 +744,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -727,23 +760,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" s="3" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
se quitaron los metodos wait, ahora lo hace por defecto
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TC1" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Locator</t>
   </si>
@@ -51,15 +51,9 @@
     <t>navigate</t>
   </si>
   <si>
-    <t xml:space="preserve">wait </t>
-  </si>
-  <si>
     <t>Screenshot</t>
   </si>
   <si>
-    <t>Wait Time</t>
-  </si>
-  <si>
     <t>xpath</t>
   </si>
   <si>
@@ -90,21 +84,6 @@
     <t>Destination Locator Value</t>
   </si>
   <si>
-    <t>dragndrop</t>
-  </si>
-  <si>
-    <t>arrastrar</t>
-  </si>
-  <si>
-    <t>http://demo.guru99.com/test/drag_drop.html</t>
-  </si>
-  <si>
-    <t>//section[@id='g-container-main']//li[4]//a[1]</t>
-  </si>
-  <si>
-    <t>//ol[@id='bank']</t>
-  </si>
-  <si>
     <t>Value Action</t>
   </si>
   <si>
@@ -121,13 +100,28 @@
   </si>
   <si>
     <t>enter</t>
+  </si>
+  <si>
+    <t>http://demo.guru99.com/test/guru99home/</t>
+  </si>
+  <si>
+    <t>clickwait</t>
+  </si>
+  <si>
+    <t>/html/body/div[1]/section/div[2]/div/div[1]/div/div[1]/div/div/div/div[2]/div[2]/div/div/div/div/div[1]/div/div/a/i</t>
+  </si>
+  <si>
+    <t>//ul[@id='flow-news']//li[5]//article[1]//a[1]//picture[1]//img[1]</t>
+  </si>
+  <si>
+    <t>numericValue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +136,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -192,7 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -201,6 +201,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -484,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,31 +507,31 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -539,7 +542,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>5</v>
@@ -558,17 +561,17 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -582,11 +585,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>3</v>
@@ -606,7 +609,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -628,7 +631,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -644,15 +647,15 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="6"/>
       <c r="E7" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -671,10 +674,10 @@
       <c r="C8" s="3"/>
       <c r="D8" s="6"/>
       <c r="E8" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -695,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,31 +709,31 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -741,10 +744,10 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -760,28 +763,26 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="J3" s="3"/>
+      <c r="J3" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -806,5 +807,6 @@
     <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se agrego documentacion(por termnar),se agrego un interfaz para la seleccion de story y test cases, ahora se abren automaticamente todos los reportes de los tc ejecutados.
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="TC1" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Locator</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Navegar a google</t>
   </si>
   <si>
-    <t>typenumeric</t>
-  </si>
-  <si>
     <t>//a[contains(text(),'Gmail')]</t>
   </si>
   <si>
@@ -94,12 +91,6 @@
   </si>
   <si>
     <t>type</t>
-  </si>
-  <si>
-    <t>//a[contains(text(),'Realeza')]</t>
-  </si>
-  <si>
-    <t>enter</t>
   </si>
   <si>
     <t>http://demo.guru99.com/test/guru99home/</t>
@@ -485,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,25 +504,25 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -561,17 +552,17 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -585,11 +576,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>3</v>
@@ -608,16 +599,16 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
+      <c r="B5" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>4</v>
+      <c r="D5" s="6"/>
+      <c r="E5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -625,66 +616,6 @@
         <v>1</v>
       </c>
       <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -698,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,25 +646,25 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -747,7 +678,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -766,23 +697,21 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="J3" s="3">
-        <v>50</v>
-      </c>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">

</xml_diff>

<commit_message>
se agrego documentacion y se arreglaron los exceptions
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="TC1" sheetId="3" r:id="rId1"/>
-    <sheet name="DragnDrop" sheetId="4" r:id="rId2"/>
+    <sheet name="Google" sheetId="5" r:id="rId2"/>
+    <sheet name="DragnDrop" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="47">
   <si>
     <t>Locator</t>
   </si>
@@ -36,15 +37,6 @@
     <t>click</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>https://www.google.com/</t>
-  </si>
-  <si>
     <t>quit</t>
   </si>
   <si>
@@ -66,15 +58,9 @@
     <t>Navegar a google</t>
   </si>
   <si>
-    <t>//a[contains(text(),'Gmail')]</t>
-  </si>
-  <si>
     <t>compto</t>
   </si>
   <si>
-    <t>Hola</t>
-  </si>
-  <si>
     <t>Destination Locator</t>
   </si>
   <si>
@@ -87,9 +73,6 @@
     <t>Value Locator</t>
   </si>
   <si>
-    <t>hola</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -102,17 +85,133 @@
     <t>/html/body/div[1]/section/div[2]/div/div[1]/div/div[1]/div/div/div/div[2]/div[2]/div/div/div/div/div[1]/div/div/a/i</t>
   </si>
   <si>
-    <t>//ul[@id='flow-news']//li[5]//article[1]//a[1]//picture[1]//img[1]</t>
-  </si>
-  <si>
     <t>numericValue</t>
+  </si>
+  <si>
+    <t>Accion</t>
+  </si>
+  <si>
+    <t>Action value</t>
+  </si>
+  <si>
+    <t>Locator Value</t>
+  </si>
+  <si>
+    <t>screenshot</t>
+  </si>
+  <si>
+    <t>Wait Time</t>
+  </si>
+  <si>
+    <t>Navigate</t>
+  </si>
+  <si>
+    <t>https://scrum-metrics.herokuapp.com/start/home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on "Get Started" </t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Getting Started')]</t>
+  </si>
+  <si>
+    <t>Click on "Login"</t>
+  </si>
+  <si>
+    <t>//button[contains(text(),'Login')]</t>
+  </si>
+  <si>
+    <t>Type username</t>
+  </si>
+  <si>
+    <t>Maria_Gonzalez</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>mat-input-0</t>
+  </si>
+  <si>
+    <t>Type password</t>
+  </si>
+  <si>
+    <t>Maria$52</t>
+  </si>
+  <si>
+    <t>mat-input-1</t>
+  </si>
+  <si>
+    <t>Click on Login</t>
+  </si>
+  <si>
+    <t>//button[@class='mat-raised-button']</t>
+  </si>
+  <si>
+    <t>Confirm</t>
+  </si>
+  <si>
+    <t>Maria Gonzalez Perez</t>
+  </si>
+  <si>
+    <t>//h1[@class='user-name']</t>
+  </si>
+  <si>
+    <t>Click on "Create a project"</t>
+  </si>
+  <si>
+    <r>
+      <t>//</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9133D4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>a[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFC75353"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>contains(text(),'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>new project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD05E07"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>')]</t>
+    </r>
+  </si>
+  <si>
+    <t>click on calendar start date</t>
+  </si>
+  <si>
+    <t>//div[@class='mat-form-field-suffix ng-tns-c15-13 ng-star-inserted']//span[@class='mat-button-wrapper']//*[local-name()='svg']//*[name()='path' and contains(@d,'M19 3h-1V1')]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,8 +233,84 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF4E4D4D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF9133D4"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFC75353"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFD05E07"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,8 +329,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -178,27 +359,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -476,13 +694,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
@@ -493,129 +711,523 @@
     <col min="10" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="H1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="C8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="11">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="11">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="J11" s="9"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="F1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="B9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="C9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="11">
         <v>9</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="B10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="3"/>
+      <c r="C10" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -625,7 +1237,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -633,52 +1245,52 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -689,7 +1301,7 @@
       </c>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -697,28 +1309,28 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3" t="b">
         <v>1</v>
       </c>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>

</xml_diff>

<commit_message>
version de prueba calendario
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="50">
   <si>
     <t>Locator</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>//div[@class='mat-form-field-suffix ng-tns-c15-13 ng-star-inserted']//span[@class='mat-button-wrapper']//*[local-name()='svg']//*[name()='path' and contains(@d,'M19 3h-1V1')]</t>
+  </si>
+  <si>
+    <t>calendar</t>
+  </si>
+  <si>
+    <t>//mat-calendar//div[contains(text(),'29')]</t>
+  </si>
+  <si>
+    <t>//div[@class='mat-checkbox-inner-container']</t>
   </si>
 </sst>
 </file>
@@ -380,7 +389,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -411,7 +420,29 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -694,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -712,255 +743,312 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="11">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="24">
+        <v>1</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="11">
+      <c r="A3" s="24">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="17" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="9"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="11">
+      <c r="A4" s="24">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="D4" s="30"/>
+      <c r="E4" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="9"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="11">
+      <c r="A5" s="24">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="9"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="11">
+      <c r="A6" s="24">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="9"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="11">
-        <v>6</v>
-      </c>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="24">
+        <v>6</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="13" t="s">
+      <c r="D7" s="30"/>
+      <c r="E7" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="9"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="23"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="11">
+      <c r="A8" s="24">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="9" t="s">
+      <c r="E8" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" s="9"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="23"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="11">
+      <c r="A9" s="24">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="20" t="s">
+      <c r="D9" s="32"/>
+      <c r="E9" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" s="9"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="23"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="11">
+      <c r="A10" s="24">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" s="23"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="35">
+        <v>10</v>
+      </c>
+      <c r="B11" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="J11" s="9"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="35">
+        <v>11</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="35">
+        <v>12</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
se agrego documetacion en driver manager y se corrigieron variables a ingles ademas de arreglar el bug de lectura.
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="TC1" sheetId="3" r:id="rId1"/>
-    <sheet name="Google" sheetId="5" r:id="rId2"/>
+    <sheet name="Google" sheetId="5" r:id="rId1"/>
+    <sheet name="TC1" sheetId="3" r:id="rId2"/>
     <sheet name="DragnDrop" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="51">
   <si>
     <t>Locator</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>//div[@class='mat-checkbox-inner-container']</t>
+  </si>
+  <si>
+    <t>Numeric Value</t>
   </si>
 </sst>
 </file>
@@ -725,10 +728,276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="11">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="11">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -739,7 +1008,7 @@
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="8" max="8" width="23.5703125" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -747,7 +1016,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>7</v>
@@ -771,7 +1040,7 @@
         <v>23</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1059,277 +1328,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="11">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="11">
-        <v>2</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="11">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="9"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="11">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="9"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="11">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="11">
-        <v>6</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="11">
-        <v>7</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="11">
-        <v>8</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="11">
-        <v>9</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
se agrego documetacion y las direcciones son relativas.
</commit_message>
<xml_diff>
--- a/excel/TC.xlsx
+++ b/excel/TC.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Google" sheetId="5" r:id="rId1"/>
+    <sheet name="TC" sheetId="5" r:id="rId1"/>
     <sheet name="TC1" sheetId="3" r:id="rId2"/>
     <sheet name="DragnDrop" sheetId="4" r:id="rId3"/>
   </sheets>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="52">
   <si>
     <t>Locator</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>Numeric Value</t>
+  </si>
+  <si>
+    <t>refresh</t>
   </si>
 </sst>
 </file>
@@ -1330,10 +1333,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1420,19 +1423,30 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>